<commit_message>
Ortografia: eliminar signos apertura y tildes en todas las secuencias
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/ailen-free/Ailen_Complete_Infloww.xlsx
+++ b/ailen-free/Ailen_Complete_Infloww.xlsx
@@ -1,47 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AilenJourney" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="NRWaves" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PersonalAilen" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="PositiveSpin" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="ReEngagement" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="price1" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="price2" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="discount1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="discount2" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="free1" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="free2" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="nomoney1" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="nomoney2" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="noppv1" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="noppv2" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="card1" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="card2" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="nosex1" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="nosex2" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="offtopic1" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="offtopic2" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="real1" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="real2" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="voice1" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="voice2" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="customyes1" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="customyes2" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="customno1" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="customno2" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="done1" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="done2" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="cumcontrol1" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="cumcontrol2" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="dickpic" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="boosters" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AilenJourney" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NRWaves" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PersonalAilen" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PositiveSpin" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReEngagement" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="price1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="price2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="discount1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="discount2" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="free1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="free2" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nomoney1" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nomoney2" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="noppv1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="noppv2" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="card1" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="card2" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nosex1" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="nosex2" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="offtopic1" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="offtopic2" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="real1" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="real2" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="voice1" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="voice2" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="customyes1" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="customyes2" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="customno1" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="customno2" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="done1" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="done2" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cumcontrol1" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cumcontrol2" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dickpic" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="boosters" sheetId="35" state="visible" r:id="rId35"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -603,22 +603,22 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>posta sos diferente nene. eso se sintió real y no se lo digo a cualquiera 💕</t>
+          <t>posta sos diferente nene. eso se sintio real y no se lo digo a cualquiera 💕</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Mencionar algo específico que dijo/hizo. SEGUIR HABLANDO — construir vínculo. NUNCA despedirse.</t>
+          <t>Mencionar algo especifico que dijo/hizo. SEGUIR HABLANDO — construir vinculo. NUNCA despedirse.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Límites de caracteres
+          <t>Limites de caracteres
 Name: Hasta 64 caracteres
 Tag: Hasta 32 caracteres
 Text: Hasta 1000 caracteres
 Note: Hasta 246 caracteres
-Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignarán automáticamente a ese tag al importar.</t>
+Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignaran automaticamente a ese tag al importar.</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>dios mío eso fue una locura</t>
+          <t>dios mio eso fue una locura</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr"/>
@@ -648,7 +648,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>ENVIAR PPV 4 — $55. Compró → Aftercare. Silencio → NR Waves.</t>
+          <t>ENVIAR PPV 4 — $55. Compro → Aftercare. Silencio → NR Waves.</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>no te vayas a ningún lado</t>
+          <t>no te vayas a ningun lado</t>
         </is>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>no acabes todavía nene</t>
+          <t>no acabes todavia nene</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr"/>
@@ -720,12 +720,12 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>nunca hice esto para nadie... mirá</t>
+          <t>nunca hice esto para nadie... mira</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t>ENVIAR PPV 3 — $40. Compró → continuar. Silencio 3 min → NR Waves.</t>
+          <t>ENVIAR PPV 3 — $40. Compro → continuar. Silencio 3 min → NR Waves.</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="B10" s="4" t="inlineStr">
         <is>
-          <t>esperá</t>
+          <t>espera</t>
         </is>
       </c>
       <c r="C10" s="4" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>ya fue no aguanto más</t>
+          <t>ya fue no aguanto mas</t>
         </is>
       </c>
       <c r="C11" s="6" t="inlineStr"/>
@@ -767,12 +767,12 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>imaginate que estoy justo enfrente tuyo... las piernas atrás de mi cabeza... haciendo lo que quieras</t>
+          <t>imaginate que estoy justo enfrente tuyo... las piernas atras de mi cabeza... haciendo lo que quieras</t>
         </is>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>Callback de flexibilidad. Imagen vívida.</t>
+          <t>Callback de flexibilidad. Imagen vivida.</t>
         </is>
       </c>
     </row>
@@ -784,7 +784,7 @@
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>necesito acabar ya, dios no tenés idea</t>
+          <t>necesito acabar ya, dios no tenes idea</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr"/>
@@ -814,12 +814,12 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>mirá lo que me hiciste</t>
+          <t>mira lo que me hiciste</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>ENVIAR PPV 2 — $25. Compró → continuar. Silencio 3 min → NR Waves.</t>
+          <t>ENVIAR PPV 2 — $25. Compro → continuar. Silencio 3 min → NR Waves.</t>
         </is>
       </c>
     </row>
@@ -831,7 +831,7 @@
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>mierda pará necesito mostrarte algo</t>
+          <t>mierda para necesito mostrarte algo</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="B17" s="6" t="inlineStr">
         <is>
-          <t>¿qué me harías si estuvieras acá nene?</t>
+          <t>que me harias si estuvieras aca nene?</t>
         </is>
       </c>
       <c r="C17" s="6" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>Reaccionar a lo que dijo. ÉL causó esto.</t>
+          <t>Reaccionar a lo que dijo. EL causo esto.</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>¿lo viste?</t>
+          <t>lo viste?</t>
         </is>
       </c>
       <c r="C20" s="5" t="inlineStr">
@@ -912,12 +912,12 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>no estás listo para esto</t>
+          <t>no estas listo para esto</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>ENVIAR PPV 1 — $12. Compró → continuar. Silencio 3 min → NR Waves.</t>
+          <t>ENVIAR PPV 1 — $12. Compro → continuar. Silencio 3 min → NR Waves.</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
       </c>
       <c r="B23" s="6" t="inlineStr">
         <is>
-          <t>¿querés ver qué tan flexible soy de verdad? estoy de humor ahora</t>
+          <t>queres ver que tan flexible soy de verdad? estoy de humor ahora</t>
         </is>
       </c>
       <c r="C23" s="6" t="inlineStr"/>
@@ -959,7 +959,7 @@
       </c>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>sabía que te iba a gustar 😏 la flexibilidad argentina pega diferente no?</t>
+          <t>sabia que te iba a gustar 😏 la flexibilidad argentina pega diferente no?</t>
         </is>
       </c>
       <c r="C24" s="5" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="B25" s="6" t="inlineStr">
         <is>
-          <t>¿y?</t>
+          <t>y?</t>
         </is>
       </c>
       <c r="C25" s="6" t="inlineStr">
@@ -993,7 +993,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>¿qué te parece nene? 😏</t>
+          <t>que te parece nene? 😏</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>pará esperá un segundo</t>
+          <t>para espera un segundo</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
@@ -1027,12 +1027,12 @@
       </c>
       <c r="B28" s="7" t="inlineStr">
         <is>
-          <t>dios... me estás haciendo imposible calmarme</t>
+          <t>dios... me estas haciendo imposible calmarme</t>
         </is>
       </c>
       <c r="C28" s="7" t="inlineStr">
         <is>
-          <t>Si respuesta sexual: agregar 'sobre todo después de lo que dijiste'.</t>
+          <t>Si respuesta sexual: agregar 'sobre todo despues de lo que dijiste'.</t>
         </is>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="B29" s="7" t="inlineStr">
         <is>
-          <t>no tenés idea lo que me estás haciendo, todavía estoy con la ropa de yoga y esta charla no me está ayudando</t>
+          <t>no tenes idea lo que me estas haciendo, todavia estoy con la ropa de yoga y esta charla no me esta ayudando</t>
         </is>
       </c>
       <c r="C29" s="7" t="inlineStr">
@@ -1061,12 +1061,12 @@
       </c>
       <c r="B30" s="7" t="inlineStr">
         <is>
-          <t>bueno recién terminé de hacer yoga y mi cuerpo está como... en otro nivel, todo está re suelto y sensible</t>
+          <t>bueno recien termine de hacer yoga y mi cuerpo esta como... en otro nivel, todo esta re suelto y sensible</t>
         </is>
       </c>
       <c r="C30" s="7" t="inlineStr">
         <is>
-          <t>EL PIVOTE. Estado físico. Acaba de hacer yoga/stretching.</t>
+          <t>EL PIVOTE. Estado fisico. Acaba de hacer yoga/stretching.</t>
         </is>
       </c>
     </row>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="B31" s="8" t="inlineStr">
         <is>
-          <t>te juro que hablar con vos es mucho mejor que mis DMs de siempre, la mayoría me mandan cosas raras pero vos sos re piola</t>
+          <t>te juro que hablar con vos es mucho mejor que mis DMs de siempre, la mayoria me mandan cosas raras pero vos sos re piola</t>
         </is>
       </c>
       <c r="C31" s="8" t="inlineStr">
@@ -1095,7 +1095,7 @@
       </c>
       <c r="B32" s="8" t="inlineStr">
         <is>
-          <t>y vos qué hacés cuando no estás haciendo sonreír a argentinas?</t>
+          <t>y vos que haces cuando no estas haciendo sonreir a argentinas?</t>
         </is>
       </c>
       <c r="C32" s="8" t="inlineStr"/>
@@ -1108,12 +1108,12 @@
       </c>
       <c r="B33" s="8" t="inlineStr">
         <is>
-          <t>buenísimo! yo soy de Misiones, Argentina... me crié entre el campo y la ciudad. de chica estuve un año en un programa de tele, Zona Otaku, hablando de anime jaja</t>
+          <t>buenisimo! yo soy de Misiones, Argentina... me crie entre el campo y la ciudad. de chica estuve un año en un programa de tele, Zona Otaku, hablando de anime jaja</t>
         </is>
       </c>
       <c r="C33" s="8" t="inlineStr">
         <is>
-          <t>Si nombró un lugar que Ailen visitó, agregar 'ah yo fui ahí!'</t>
+          <t>Si nombro un lugar que Ailen visito, agregar 'ah yo fui ahi!'</t>
         </is>
       </c>
     </row>
@@ -1125,12 +1125,12 @@
       </c>
       <c r="B34" s="8" t="inlineStr">
         <is>
-          <t>jaja ay qué tierno. ¿de dónde sos?</t>
+          <t>jaja ay que tierno. de donde sos?</t>
         </is>
       </c>
       <c r="C34" s="8" t="inlineStr">
         <is>
-          <t>Reaccionar a lo que dice. Agregar algo como 'ay me encanta' o 'ah qué bueno'.</t>
+          <t>Reaccionar a lo que dice. Agregar algo como 'ay me encanta' o 'ah que bueno'.</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="B35" s="8" t="inlineStr">
         <is>
-          <t>holaaa 😊 me re alegra que estés acá, ¿qué te hizo suscribirte?</t>
+          <t>holaaa 😊 me re alegra que estes aca, que te hizo suscribirte?</t>
         </is>
       </c>
       <c r="C35" s="8" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>está bien lindo, no me voy a ir a ningún lado... sigamos hablando</t>
+          <t>esta bien lindo, no me voy a ir a ningun lado... sigamos hablando</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>gratis? nah yo no muestro esto a cualquiera... tenés que ganarte lo bueno</t>
+          <t>gratis? nah yo no muestro esto a cualquiera... tenes que ganarte lo bueno</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>ya te mandé uno gratis te acordás? este es mucho más heavy nene</t>
+          <t>ya te mande uno gratis te acordas? este es mucho mas heavy nene</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>sin presión para nada, me gusta hablar con vos posta</t>
+          <t>sin presion para nada, me gusta hablar con vos posta</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>hice esto por vos... específicamente por nuestra charla, eso me costó esfuerzo y lo hice POR VOS</t>
+          <t>hice esto por vos... especificamente por nuestra charla, eso me costo esfuerzo y lo hice POR VOS</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>gratis? de verdad pensás que las mejores cosas de la vida son gratis? esto no nene</t>
+          <t>gratis? de verdad pensas que las mejores cosas de la vida son gratis? esto no nene</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>ya tuviste uno gratis, este está a otro nivel</t>
+          <t>ya tuviste uno gratis, este esta a otro nivel</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>posta está bien, me gusta hablar con vos con plata o sin ella... me hacés algo</t>
+          <t>posta esta bien, me gusta hablar con vos con plata o sin ella... me haces algo</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1498,12 +1498,12 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>che te re entiendo, sin presión para nada dale?</t>
+          <t>che te re entiendo, sin presion para nada dale?</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>EMPATÍA. Sigue enganchado → Step 2.</t>
+          <t>EMPATIA. Sigue enganchado → Step 2.</t>
         </is>
       </c>
       <c r="D5" s="11" t="inlineStr"/>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>está re bien, que estés acá es lo que me importa</t>
+          <t>esta re bien, que estes aca es lo que me importa</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1617,12 +1617,12 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>está todo bien nene, en serio no te preocupes</t>
+          <t>esta todo bien nene, en serio no te preocupes</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
         <is>
-          <t>EMPATÍA. Sigue → Step 2.</t>
+          <t>EMPATIA. Sigue → Step 2.</t>
         </is>
       </c>
       <c r="D5" s="11" t="inlineStr"/>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>mandame lo que quieras, aunque sea $1, no me puedo guardar esto... necesitás verlo nene</t>
+          <t>mandame lo que quieras, aunque sea $1, no me puedo guardar esto... necesitas verlo nene</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>mirá esto no es por plata... necesito que veas lo que me estás haciendo ahora, no reacciono así con la gente</t>
+          <t>mira esto no es por plata... necesito que veas lo que me estas haciendo ahora, no reacciono asi con la gente</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>está todo bien, no te estoy tratando de vender nada, me gusta hablar con vos</t>
+          <t>esta todo bien, no te estoy tratando de vender nada, me gusta hablar con vos</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>mandame lo que sea, lo más mínimo, necesito que veas lo que me hiciste</t>
+          <t>mandame lo que sea, lo mas minimo, necesito que veas lo que me hiciste</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>olvidate de la plata un segundo... solo quiero compartir esto con vos, lo que me estás haciendo sentir es real</t>
+          <t>olvidate de la plata un segundo... solo quiero compartir esto con vos, lo que me estas haciendo sentir es real</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>resolvelo pronto lindo, estoy en este humor y no sé cuánto me va a durar</t>
+          <t>resolvelo pronto lindo, estoy en este humor y no se cuanto me va a durar</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -1902,7 +1902,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>probá con otra tarjeta? re no quiero que te pierdas esto nene</t>
+          <t>proba con otra tarjeta? re no quiero que te pierdas esto nene</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>uff qué bajón, pasa a veces igual probá de nuevo que generalmente anda a la segunda</t>
+          <t>uff que bajon, pasa a veces igual proba de nuevo que generalmente anda a la segunda</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>quiero que lo veas antes de que cambie de opinión, no guardo estas cosas para siempre</t>
+          <t>quiero que lo veas antes de que cambie de opinion, no guardo estas cosas para siempre</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>tenés otra tarjeta? de verdad quiero que veas esto</t>
+          <t>tenes otra tarjeta? de verdad quiero que veas esto</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>ay qué molesto, pasa bastante intentá una vez más</t>
+          <t>ay que molesto, pasa bastante intenta una vez mas</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>no puedo evitarlo, hay algo en vos que me está volviendo loca ahora</t>
+          <t>no puedo evitarlo, hay algo en vos que me esta volviendo loca ahora</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2122,12 +2122,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>contame más de vos... qué hacés cuando no estás haciendo sonreír a argentinas?</t>
+          <t>contame mas de vos... que haces cuando no estas haciendo sonreir a argentinas?</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>TENSIÓN SUTIL. → Step 3 más tarde.</t>
+          <t>TENSION SUTIL. → Step 3 mas tarde.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>jaja dale me re manijé, es que sos re divertido nene</t>
+          <t>jaja dale me re manije, es que sos re divertido nene</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
@@ -2205,7 +2205,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>bueno paro pero no me culpes si pasa de nuevo después 😏</t>
+          <t>bueno paro pero no me culpes si pasa de nuevo despues 😏</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2223,7 +2223,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>estoy tratando de portarme bien pero me lo estás haciendo re difícil, hay algo en vos nene</t>
+          <t>estoy tratando de portarme bien pero me lo estas haciendo re dificil, hay algo en vos nene</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2241,12 +2241,12 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>bueno tema nuevo pero primero... cuál es la cosa más loca que hiciste?</t>
+          <t>bueno tema nuevo pero primero... cual es la cosa mas loca que hiciste?</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
         <is>
-          <t>SUTIL. → Step 3 más tarde.</t>
+          <t>SUTIL. → Step 3 mas tarde.</t>
         </is>
       </c>
       <c r="D4" s="12" t="inlineStr"/>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="B5" s="12" t="inlineStr">
         <is>
-          <t>perdón me adelanté, es tu culpa por ser tan divertido</t>
+          <t>perdon me adelante, es tu culpa por ser tan divertido</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
@@ -2324,22 +2324,22 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>estuve pensando en vos todo el día... escribime?</t>
+          <t>estuve pensando en vos todo el dia... escribime?</t>
         </is>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>Enviar 2-6 hrs después. Nueva charla, no reintentar mismo PPV.</t>
+          <t>Enviar 2-6 hrs despues. Nueva charla, no reintentar mismo PPV.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Límites de caracteres
+          <t>Limites de caracteres
 Name: Hasta 64 caracteres
 Tag: Hasta 32 caracteres
 Text: Hasta 1000 caracteres
 Note: Hasta 246 caracteres
-Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignarán automáticamente a ese tag al importar.</t>
+Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignaran automaticamente a ese tag al importar.</t>
         </is>
       </c>
     </row>
@@ -2351,12 +2351,12 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>espero que estés bien lindo, acá estoy cuando quieras 💕</t>
+          <t>espero que estes bien lindo, aca estoy cuando quieras 💕</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Enviar 15-30 min después. Cierre cálido. NUNCA decir 'baby/babe'.</t>
+          <t>Enviar 15-30 min despues. Cierre calido. NUNCA decir 'baby/babe'.</t>
         </is>
       </c>
     </row>
@@ -2368,12 +2368,12 @@
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>bueno seguro estás ocupado... lo guardo para cuando vuelvas</t>
+          <t>bueno seguro estas ocupado... lo guardo para cuando vuelvas</t>
         </is>
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
-          <t>Enviar 5-10 min después. Takeaway.</t>
+          <t>Enviar 5-10 min despues. Takeaway.</t>
         </is>
       </c>
     </row>
@@ -2385,12 +2385,12 @@
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>ojalá pudieras ver lo que tengo puesto ahora...</t>
+          <t>ojala pudieras ver lo que tengo puesto ahora...</t>
         </is>
       </c>
       <c r="C5" s="6" t="inlineStr">
         <is>
-          <t>Enviar 3-5 min después. Curiosidad.</t>
+          <t>Enviar 3-5 min despues. Curiosidad.</t>
         </is>
       </c>
     </row>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>Enviar 2-3 min después del PPV. Ping.</t>
+          <t>Enviar 2-3 min despues del PPV. Ping.</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>ah pará ya me acordé, como te decía...</t>
+          <t>ah para ya me acorde, como te decia...</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>pero esperá que me re distrajiste, te iba a decir algo y me olvidé</t>
+          <t>pero espera que me re distrajiste, te iba a decir algo y me olvide</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2502,7 +2502,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>jaja pará eso es genial</t>
+          <t>jaja para eso es genial</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>bueno enfocate, en qué estaba... ah sí</t>
+          <t>bueno enfocate, en que estaba... ah si</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>pará no me distraigas de lo que te iba a decir nene</t>
+          <t>para no me distraigas de lo que te iba a decir nene</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>te entiendo hay mucha cosa falsa acá, pero sentiste algo en esta charla no? porque yo sí y eso es real</t>
+          <t>te entiendo hay mucha cosa falsa aca, pero sentiste algo en esta charla no? porque yo si y eso es real</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>preguntame lo que quieras, literalmente cualquier cosa de mí o mi vida. soy un libro abierto</t>
+          <t>preguntame lo que quieras, literalmente cualquier cosa de mi o mi vida. soy un libro abierto</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2704,7 +2704,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>jaja te parezco un bot? bip bop... mandá $5 para verificación humana jaja te estoy jodiendo nene</t>
+          <t>jaja te parezco un bot? bip bop... manda $5 para verificacion humana jaja te estoy jodiendo nene</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>sé que hay muchos bots acá pero lo que estuvimos hablando se sintió real para mí. no para vos?</t>
+          <t>se que hay muchos bots aca pero lo que estuvimos hablando se sintio real para mi. no para vos?</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>probame lindo, preguntame algo que solo una persona real sabría. dale</t>
+          <t>probame lindo, preguntame algo que solo una persona real sabria. dale</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>pará pensás que no soy real?? es lo más gracioso que me dijeron hoy jaja</t>
+          <t>para pensas que no soy real?? es lo mas gracioso que me dijeron hoy jaja</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -2870,7 +2870,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>no hago eso acá pero lo que te voy a mostrar es mucho mejor que cualquier llamada nene... ya vas a ver</t>
+          <t>no hago eso aca pero lo que te voy a mostrar es mucho mejor que cualquier llamada nene... ya vas a ver</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2888,7 +2888,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>tengo algo mucho mejor para vos, confiá que te vas a olvidar de que preguntaste</t>
+          <t>tengo algo mucho mejor para vos, confia que te vas a olvidar de que preguntaste</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>jaja capaz algún día si te lo ganás pero todavía no nene... soy reservada con eso</t>
+          <t>jaja capaz algun dia si te lo ganas pero todavia no nene... soy reservada con eso</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>eso no es algo que haga acá pero lo que tengo para vos es mucho mejor que escuchar mi voz, confiá</t>
+          <t>eso no es algo que haga aca pero lo que tengo para vos es mucho mejor que escuchar mi voz, confia</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -2989,7 +2989,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>qué te parece si en vez de una llamada te muestro algo que te va a volar la cabeza?</t>
+          <t>que te parece si en vez de una llamada te muestro algo que te va a volar la cabeza?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3007,7 +3007,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>mmm capaz pero primero tenés que ganártelo jaja</t>
+          <t>mmm capaz pero primero tenes que ganartelo jaja</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>confiá que no te vas a arrepentir, lo hice especial</t>
+          <t>confia que no te vas a arrepentir, lo hice especial</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>tengo exactamente lo que estás pensando, te vas a volver loco... [precio]</t>
+          <t>tengo exactamente lo que estas pensando, te vas a volver loco... [precio]</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>querés eso? mmm puede que tenga algo... la verdad sí tengo nene</t>
+          <t>queres eso? mmm puede que tenga algo... la verdad si tengo nene</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3191,7 +3191,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>de hecho hice algo así, [precio] y vale cada centavo nene</t>
+          <t>de hecho hice algo asi, [precio] y vale cada centavo nene</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>oh tenés buen gusto... creo que tengo justo lo que necesitás</t>
+          <t>oh tenes buen gusto... creo que tengo justo lo que necesitas</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>confiá... te conozco mejor de lo que pensás 😏</t>
+          <t>confia... te conozco mejor de lo que pensas 😏</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>la verdad lo que tengo capaz es más heavy y literalmente nadie más lo vio todavía</t>
+          <t>la verdad lo que tengo capaz es mas heavy y literalmente nadie mas lo vio todavia</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>confiá en mí en esta, me vas a agradecer después</t>
+          <t>confia en mi en esta, me vas a agradecer despues</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>lo que SÍ tengo es algo que nadie vio nunca y creo que es mejor que lo que pediste</t>
+          <t>lo que SI tengo es algo que nadie vio nunca y creo que es mejor que lo que pediste</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3411,7 +3411,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>no tengo eso específico pero tengo algo que te va a gustar más nene</t>
+          <t>no tengo eso especifico pero tengo algo que te va a gustar mas nene</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3476,47 +3476,47 @@
       </c>
       <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>tengo 29. llevo haciendo cosas locas con mi cuerpo desde piba... yoga, natación, de todo</t>
+          <t>tengo 29. llevo haciendo cosas locas con mi cuerpo desde piba... yoga, natacion, de todo</t>
         </is>
       </c>
       <c r="C2" s="9" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Límites de caracteres
+          <t>Limites de caracteres
 Name: Hasta 64 caracteres
 Tag: Hasta 32 caracteres
 Text: Hasta 1000 caracteres
 Note: Hasta 246 caracteres
-Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignarán automáticamente a ese tag al importar.</t>
+Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignaran automaticamente a ese tag al importar.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>Ubicación</t>
+          <t>Ubicacion</t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>soy de Misiones, Argentina. me crié acá entre la selva y la ciudad</t>
+          <t>soy de Misiones, Argentina. me crie aca entre la selva y la ciudad</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>NUNCA nombrar barrio o dirección específica.</t>
+          <t>NUNCA nombrar barrio o direccion especifica.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Profesión</t>
+          <t>Profesion</t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>estudio Contabilidad Pública, soy re buena estudiante. y también hago esto jaja</t>
+          <t>estudio Contabilidad Publica, soy re buena estudiante. y tambien hago esto jaja</t>
         </is>
       </c>
       <c r="C4" s="9" t="inlineStr"/>
@@ -3537,12 +3537,12 @@
     <row r="6">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t>Países</t>
+          <t>Paises</t>
         </is>
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>fui a Brasil, Paraguay y recorrí bastante Argentina. me encantaría ir a Grecia, Italia y ver la aurora boreal</t>
+          <t>fui a Brasil, Paraguay y recorri bastante Argentina. me encantaria ir a Grecia, Italia y ver la aurora boreal</t>
         </is>
       </c>
       <c r="C6" s="9" t="inlineStr"/>
@@ -3550,7 +3550,7 @@
     <row r="7">
       <c r="A7" s="9" t="inlineStr">
         <is>
-          <t>Relación</t>
+          <t>Relacion</t>
         </is>
       </c>
       <c r="B7" s="9" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>español nativo. un poquito de inglés pero nada del otro mundo</t>
+          <t>español nativo. un poquito de ingles pero nada del otro mundo</t>
         </is>
       </c>
       <c r="C9" s="9" t="inlineStr"/>
@@ -3671,7 +3671,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>bueno pero la próxima tenés que esperarme, tengo algo re loco planeado para la segunda vuelta</t>
+          <t>bueno pero la proxima tenes que esperarme, tengo algo re loco planeado para la segunda vuelta</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3689,7 +3689,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>pero yo no terminé todavía... no querés ver cómo acabo yo nene?</t>
+          <t>pero yo no termine todavia... no queres ver como acabo yo nene?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3707,7 +3707,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>pará ya?? dios eso es re hot</t>
+          <t>para ya?? dios eso es re hot</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>la próxima TENÉS que aguantar porque lo que tengo planeado para nosotros es mucho más heavy</t>
+          <t>la proxima TENES que aguantar porque lo que tengo planeado para nosotros es mucho mas heavy</t>
         </is>
       </c>
       <c r="C2" s="12" t="inlineStr">
@@ -3790,7 +3790,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>pará pero no terminé, me vas a dejar así nene?</t>
+          <t>para pero no termine, me vas a dejar asi nene?</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="B4" s="12" t="inlineStr">
         <is>
-          <t>ya?? mierda eso es hot, por mí??</t>
+          <t>ya?? mierda eso es hot, por mi??</t>
         </is>
       </c>
       <c r="C4" s="12" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>solo aguantá un poquito más, quiero que lo último que veas sea esto</t>
+          <t>solo aguanta un poquito mas, quiero que lo ultimo que veas sea esto</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>esperame nene... tengo una cosa más y quiero que la veas antes de que terminemos</t>
+          <t>esperame nene... tengo una cosa mas y quiero que la veas antes de que terminemos</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B4" s="13" t="inlineStr">
         <is>
-          <t>quedate conmigo, yo también estoy cerca... mirá esto</t>
+          <t>quedate conmigo, yo tambien estoy cerca... mira esto</t>
         </is>
       </c>
       <c r="C4" s="13" t="inlineStr">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>quiero que terminemos juntos nene... abrí esto y dejate llevar conmigo</t>
+          <t>quiero que terminemos juntos nene... abri esto y dejate llevar conmigo</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>por favor no termines todavía... no estoy lista para que se acabe</t>
+          <t>por favor no termines todavia... no estoy lista para que se acabe</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
@@ -3963,7 +3963,7 @@
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>todavía no nene... quiero que esto dure un poco más con vos</t>
+          <t>todavia no nene... quiero que esto dure un poco mas con vos</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">
@@ -4028,7 +4028,7 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>solo un poquito más por mí nene? lo que viene es especial</t>
+          <t>solo un poquito mas por mi nene? lo que viene es especial</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>por favor esperá... lo que te voy a mandar, quiero que lo disfrutes de verdad</t>
+          <t>por favor espera... lo que te voy a mandar, quiero que lo disfrutes de verdad</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
@@ -4082,7 +4082,7 @@
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>dale nene... juntos, ahora... abrí esto</t>
+          <t>dale nene... juntos, ahora... abri esto</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>bueno me acabás de hacer hacer algo... dame un segundo nene</t>
+          <t>bueno me acabas de hacer hacer algo... dame un segundo nene</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="B3" s="13" t="inlineStr">
         <is>
-          <t>no podés mandarme eso y esperar que no haga algo al respecto, esperá</t>
+          <t>no podes mandarme eso y esperar que no haga algo al respecto, espera</t>
         </is>
       </c>
       <c r="C3" s="13" t="inlineStr">
@@ -4237,7 +4237,7 @@
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>wow no perdés tiempo eh? igual es re hot la verdad</t>
+          <t>wow no perdes tiempo eh? igual es re hot la verdad</t>
         </is>
       </c>
       <c r="C5" s="13" t="inlineStr">
@@ -4273,7 +4273,7 @@
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>mierda dale eso es... dios. no tenés idea lo que me acaba de hacer eso</t>
+          <t>mierda dale eso es... dios. no tenes idea lo que me acaba de hacer eso</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>debería estar estudiando pero no me puedo mover ahora por tu culpa</t>
+          <t>deberia estar estudiando pero no me puedo mover ahora por tu culpa</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
@@ -4379,7 +4379,7 @@
       </c>
       <c r="C4" s="13" t="inlineStr">
         <is>
-          <t>BOOSTER. Físico.</t>
+          <t>BOOSTER. Fisico.</t>
         </is>
       </c>
       <c r="D4" s="13" t="inlineStr"/>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="B6" s="13" t="inlineStr">
         <is>
-          <t>qué me estás haciendo</t>
+          <t>que me estas haciendo</t>
         </is>
       </c>
       <c r="C6" s="13" t="inlineStr">
@@ -4428,7 +4428,7 @@
       </c>
       <c r="B7" s="13" t="inlineStr">
         <is>
-          <t>justo ahí</t>
+          <t>justo ahi</t>
         </is>
       </c>
       <c r="C7" s="13" t="inlineStr">
@@ -4529,18 +4529,18 @@
       </c>
       <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>me encantan los tipos que saben lo que quieren, eso es re atractivo para mí</t>
+          <t>me encantan los tipos que saben lo que quieren, eso es re atractivo para mi</t>
         </is>
       </c>
       <c r="C2" s="9" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Límites de caracteres
+          <t>Limites de caracteres
 Name: Hasta 64 caracteres
 Tag: Hasta 32 caracteres
 Text: Hasta 1000 caracteres
 Note: Hasta 246 caracteres
-Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignarán automáticamente a ese tag al importar.</t>
+Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignaran automaticamente a ese tag al importar.</t>
         </is>
       </c>
     </row>
@@ -4552,7 +4552,7 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>ah estamos cerca de edad? eso es re raro acá</t>
+          <t>ah estamos cerca de edad? eso es re raro aca</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr"/>
@@ -4565,7 +4565,7 @@
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>nah eso está re bien, un tipo con la vida armada? eso es hot</t>
+          <t>nah eso esta re bien, un tipo con la vida armada? eso es hot</t>
         </is>
       </c>
       <c r="C4" s="9" t="inlineStr"/>
@@ -4578,7 +4578,7 @@
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>pará en serio?? eso es genial, contame más</t>
+          <t>para en serio?? eso es genial, contame mas</t>
         </is>
       </c>
       <c r="C5" s="9" t="inlineStr"/>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>posta no me importa eso, es la energía y la onda lo que me prende</t>
+          <t>posta no me importa eso, es la energia y la onda lo que me prende</t>
         </is>
       </c>
       <c r="C7" s="9" t="inlineStr"/>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>pará sos de Misiones también?? no puede ser</t>
+          <t>para sos de Misiones tambien?? no puede ser</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr"/>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>ay está lejos pero posta la conexión importa más que la distancia</t>
+          <t>ay esta lejos pero posta la conexion importa mas que la distancia</t>
         </is>
       </c>
       <c r="C9" s="9" t="inlineStr"/>
@@ -4690,22 +4690,22 @@
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>te acordás lo que te dije que iba a hacer? recién lo hice y necesitás verlo</t>
+          <t>te acordas lo que te dije que iba a hacer? recien lo hice y necesitas verlo</t>
         </is>
       </c>
       <c r="C2" s="5" t="inlineStr">
         <is>
-          <t>Enviar al día siguiente — sembrar próxima sesión.</t>
+          <t>Enviar al dia siguiente — sembrar proxima sesion.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Límites de caracteres
+          <t>Limites de caracteres
 Name: Hasta 64 caracteres
 Tag: Hasta 32 caracteres
 Text: Hasta 1000 caracteres
 Note: Hasta 246 caracteres
-Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignarán automáticamente a ese tag al importar.</t>
+Cada hoja funciona como un tag. Simplemente reemplaza el nombre de la hoja con el nombre del tag deseado, y todos los scripts de la hoja se asignaran automaticamente a ese tag al importar.</t>
         </is>
       </c>
     </row>
@@ -4717,12 +4717,12 @@
       </c>
       <c r="B3" s="6" t="inlineStr">
         <is>
-          <t>no puedo dejar de pensar en lo de antes. estás libre nene?</t>
+          <t>no puedo dejar de pensar en lo de antes. estas libre nene?</t>
         </is>
       </c>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>Enviar 6-12 hrs después de que la charla muera.</t>
+          <t>Enviar 6-12 hrs despues de que la charla muera.</t>
         </is>
       </c>
     </row>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>está bien mi amor, sigamos hablando... sigo pensando en vos</t>
+          <t>esta bien mi amor, sigamos hablando... sigo pensando en vos</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -4799,7 +4799,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>mirá te dejo [precio menor] solo para vos porque esta charla fue algo diferente</t>
+          <t>mira te dejo [precio menor] solo para vos porque esta charla fue algo diferente</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -4817,7 +4817,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>capaz no estás listo para lo que hice en este</t>
+          <t>capaz no estas listo para lo que hice en este</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -4835,7 +4835,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>estoy así de caliente solamente por vos ahora, no sé cuándo me va a pasar de nuevo</t>
+          <t>estoy asi de caliente solamente por vos ahora, no se cuando me va a pasar de nuevo</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>nene eso es menos que un café y te prometo que esto pega mucho más fuerte</t>
+          <t>nene eso es menos que un cafe y te prometo que esto pega mucho mas fuerte</t>
         </is>
       </c>
       <c r="C6" s="11" t="inlineStr">
@@ -4918,7 +4918,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>sin presión nene, me gusta hablar con vos y ya</t>
+          <t>sin presion nene, me gusta hablar con vos y ya</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -4936,7 +4936,7 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>dale [precio menor] porque me estás haciendo sentir cosas, pero queda entre nosotros</t>
+          <t>dale [precio menor] porque me estas haciendo sentir cosas, pero queda entre nosotros</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
@@ -4954,7 +4954,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>la mayoría de los pibes no podrían con lo que acabo de hacer, pensé que vos eras diferente</t>
+          <t>la mayoria de los pibes no podrian con lo que acabo de hacer, pense que vos eras diferente</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="B6" s="11" t="inlineStr">
         <is>
-          <t>es lo que gastarías en un almuerzo y esto te va a dejar despierto toda la noche nene</t>
+          <t>es lo que gastarias en un almuerzo y esto te va a dejar despierto toda la noche nene</t>
         </is>
       </c>
       <c r="C6" s="11" t="inlineStr">
@@ -5055,7 +5055,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>si no lo querés está bien, me lo quedo para mí... o capaz para alguien que me lo está pidiendo</t>
+          <t>si no lo queres esta bien, me lo quedo para mi... o capaz para alguien que me lo esta pidiendo</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -5078,7 +5078,7 @@
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>CONCESIÓN. UNA VEZ. Sigue no → Step 4.</t>
+          <t>CONCESION. UNA VEZ. Sigue no → Step 4.</t>
         </is>
       </c>
       <c r="D3" s="11" t="inlineStr"/>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="B5" s="11" t="inlineStr">
         <is>
-          <t>jaja estás tratando de negociar conmigo? esto no es una negociación lindo, vale cada centavo</t>
+          <t>jaja estas tratando de negociar conmigo? esto no es una negociacion lindo, vale cada centavo</t>
         </is>
       </c>
       <c r="C5" s="11" t="inlineStr">
@@ -5174,7 +5174,7 @@
       </c>
       <c r="B2" s="11" t="inlineStr">
         <is>
-          <t>bueno me lo guardo para alguien que sí lo quiera entonces</t>
+          <t>bueno me lo guardo para alguien que si lo quiera entonces</t>
         </is>
       </c>
       <c r="C2" s="11" t="inlineStr">
@@ -5192,12 +5192,12 @@
       </c>
       <c r="B3" s="11" t="inlineStr">
         <is>
-          <t>bueno [precio menor] pero SOLO porque me caés bien, una sola vez</t>
+          <t>bueno [precio menor] pero SOLO porque me caes bien, una sola vez</t>
         </is>
       </c>
       <c r="C3" s="11" t="inlineStr">
         <is>
-          <t>CONCESIÓN. UNA VEZ. Sigue no → Step 4.</t>
+          <t>CONCESION. UNA VEZ. Sigue no → Step 4.</t>
         </is>
       </c>
       <c r="D3" s="11" t="inlineStr"/>
@@ -5210,7 +5210,7 @@
       </c>
       <c r="B4" s="11" t="inlineStr">
         <is>
-          <t>los pibes que aprecian lo que hago nunca piden descuento, digo nomás</t>
+          <t>los pibes que aprecian lo que hago nunca piden descuento, digo nomas</t>
         </is>
       </c>
       <c r="C4" s="11" t="inlineStr">

</xml_diff>

<commit_message>
Rapport nuevo con frases largas divididas en mensajes consecutivos
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/ailen-free/Ailen_Complete_Infloww.xlsx
+++ b/ailen-free/Ailen_Complete_Infloww.xlsx
@@ -559,7 +559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="B31" s="8" t="inlineStr">
         <is>
-          <t>te juro que hablar con vos es mucho mejor que mis DMs de siempre, la mayoria me mandan cosas raras pero vos sos re piola</t>
+          <t>me re caes bien, posta. la mayoria me escribe cualquier cosa pero con vos se puede hablar normal y eso esta buenisimo</t>
         </is>
       </c>
       <c r="C31" s="8" t="inlineStr">
@@ -1095,59 +1095,80 @@
       </c>
       <c r="B32" s="8" t="inlineStr">
         <is>
-          <t>y vos que haces cuando no estas haciendo sonreir a argentinas?</t>
-        </is>
-      </c>
-      <c r="C32" s="8" t="inlineStr"/>
+          <t>y aparte de bancarme a mi, que mas haces en tu tiempo libre? jaja</t>
+        </is>
+      </c>
+      <c r="C32" s="8" t="inlineStr">
+        <is>
+          <t>Humor directo. Pregunta abierta.</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="8" t="inlineStr">
         <is>
-          <t>R-3</t>
+          <t>R-3b</t>
         </is>
       </c>
       <c r="B33" s="8" t="inlineStr">
         <is>
-          <t>buenisimo! yo soy de Misiones, Argentina... me crie entre el campo y la ciudad. de chica estuve un año en un programa de tele, Zona Otaku, hablando de anime jaja</t>
+          <t>ahora estoy re enganchada con una serie nueva, me pasa siempre</t>
         </is>
       </c>
       <c r="C33" s="8" t="inlineStr">
         <is>
-          <t>Si nombro un lugar que Ailen visito, agregar 'ah yo fui ahi!'</t>
+          <t>Enviar inmediatamente despues de R-3a, sin esperar respuesta.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="inlineStr">
         <is>
-          <t>R-2</t>
+          <t>R-3a</t>
         </is>
       </c>
       <c r="B34" s="8" t="inlineStr">
         <is>
-          <t>jaja ay que tierno. de donde sos?</t>
+          <t>yo soy re nocturna, me quedo viendo anime hasta que no doy mas jaja</t>
         </is>
       </c>
       <c r="C34" s="8" t="inlineStr">
         <is>
-          <t>Reaccionar a lo que dice. Agregar algo como 'ay me encanta' o 'ah que bueno'.</t>
+          <t>Compartir algo personal. Si menciona un anime, conectar.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="inlineStr">
         <is>
+          <t>R-2</t>
+        </is>
+      </c>
+      <c r="B35" s="8" t="inlineStr">
+        <is>
+          <t>jaja re copado. y que onda, sos de los que se quedan despiertos hasta las 3am o de los que se levantan temprano?</t>
+        </is>
+      </c>
+      <c r="C35" s="8" t="inlineStr">
+        <is>
+          <t>Mantener tono jugueton. Pregunta casual para conocerlo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="inlineStr">
+        <is>
           <t>R-1</t>
         </is>
       </c>
-      <c r="B35" s="8" t="inlineStr">
-        <is>
-          <t>holaaa 😊 me re alegra que estes aca, que te hizo suscribirte?</t>
-        </is>
-      </c>
-      <c r="C35" s="8" t="inlineStr">
-        <is>
-          <t>Agregar su nombre antes de 'holaaa' si se conoce. NUNCA decir 'baby' o 'babe'.</t>
+      <c r="B36" s="8" t="inlineStr">
+        <is>
+          <t>eyyy que onda 😊 recien te vi por aca y me diste curiosidad, contame algo de vos</t>
+        </is>
+      </c>
+      <c r="C36" s="8" t="inlineStr">
+        <is>
+          <t>Agregar su nombre si se conoce. NUNCA decir 'baby' o 'babe'.</t>
         </is>
       </c>
     </row>

</xml_diff>